<commit_message>
Changes to protocol to modify IC dispense. Dot well figure creator.
</commit_message>
<xml_diff>
--- a/Automation/base_scripts/Reference_template.xlsx
+++ b/Automation/base_scripts/Reference_template.xlsx
@@ -221,7 +221,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,6 +270,42 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="21"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="23"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="24"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="25"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="26"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="48">
     <border>
@@ -1083,13 +1119,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1104,7 +1140,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="8" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1128,7 +1164,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="8" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="37" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1137,34 +1173,34 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="32" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="9" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="7" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1176,40 +1212,40 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="11" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="11" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1227,7 +1263,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="40" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="40" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1236,7 +1272,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="42" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="43" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="43" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1245,7 +1281,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="45" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="46" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="46" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1279,13 +1315,19 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffccfcac"/>
+      <rgbColor rgb="ff4dac2b"/>
       <rgbColor rgb="ff0432ff"/>
-      <rgbColor rgb="ffff8cc5"/>
-      <rgbColor rgb="fffcde9e"/>
-      <rgbColor rgb="ffa6daff"/>
+      <rgbColor rgb="ffff0800"/>
+      <rgbColor rgb="fffae232"/>
+      <rgbColor rgb="ff006fff"/>
       <rgbColor rgb="ffa7b7ff"/>
+      <rgbColor rgb="fffcf500"/>
+      <rgbColor rgb="ffff1900"/>
+      <rgbColor rgb="ff0064ff"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffff2200"/>
+      <rgbColor rgb="fff1fc00"/>
+      <rgbColor rgb="ff006aff"/>
     </indexedColors>
   </colors>
 </styleSheet>

</xml_diff>